<commit_message>
finished scraping for wwe championship
</commit_message>
<xml_diff>
--- a/wwe-champions/column-template.xlsx
+++ b/wwe-champions/column-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f11b2f436f06de33/github/kaggle-non-competition/wwe-champions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\OneDrive\github\kaggle-non-competition\wwe-champions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{4DED31FC-85E6-4624-9C5D-8CB857F54DA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2AC6876A-423C-469B-A6BF-1158F3936969}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{4DED31FC-85E6-4624-9C5D-8CB857F54DA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{912F4334-CD47-423C-8A4A-A4FA2ABED536}"/>
   <bookViews>
-    <workbookView xWindow="19350" yWindow="435" windowWidth="18720" windowHeight="20490" xr2:uid="{E4270448-793E-428D-B71D-5383FBEC75C3}"/>
+    <workbookView xWindow="18240" yWindow="795" windowWidth="18720" windowHeight="20490" xr2:uid="{E4270448-793E-428D-B71D-5383FBEC75C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,10 +70,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,8 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA1DC31-C710-4609-B135-6F3CF05B6CE7}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +458,7 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F1" t="s">
@@ -451,13 +467,13 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="K1" t="s">
@@ -466,5 +482,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>